<commit_message>
[1W-2] Done lect1 hw3~7
- Understood changes of memory and register by following codes
- Compared C-code with ASM code
- hw8 is in progress (needs to question to Prof. about 'leave')
</commit_message>
<xml_diff>
--- a/lect01_hw3_memory map.xlsx
+++ b/lect01_hw3_memory map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\윤성호\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inha0-my.sharepoint.com/personal/12161756_inha_edu/Documents/Git/Information_Security/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A9945-A229-40C2-805E-F4872CD8B0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{BD0A9945-A229-40C2-805E-F4872CD8B0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46DC22B3-7686-42F9-B730-BCC8BE93DD69}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA8BD21B-3500-4B17-94FF-5435036B4A47}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="104">
   <si>
     <t>bffff63c</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -390,39 +390,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>80482f0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>⑪ leave</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>80482f1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>80482f2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>80482f5</t>
-  </si>
-  <si>
-    <t>80482f4</t>
-  </si>
-  <si>
-    <t>80482f3</t>
-  </si>
-  <si>
     <t>⑫ ret</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -456,6 +427,10 @@
   </si>
   <si>
     <t>⑧ mov DWORD PTR[esp+0x4], eax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -718,15 +693,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -761,6 +727,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -988,8 +963,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6731877" y="593835"/>
-          <a:ext cx="0" cy="1266496"/>
+          <a:off x="6715184" y="597545"/>
+          <a:ext cx="0" cy="1285352"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2218,6 +2193,658 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>412377</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>412377</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>57187</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="직선 화살표 연결선 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6398279C-0607-4D6A-9ECB-B5E79D80F6B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="690283" y="21120847"/>
+          <a:ext cx="0" cy="819187"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>233701</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>192278</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>596308</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>22567</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="타원 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A999F8D-6276-4CF0-9B17-5BE6F8B70B7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1354289" y="21178654"/>
+          <a:ext cx="362607" cy="959842"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>543205</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>115083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>439270</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="직선 화살표 연결선 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1B85B2D-5EC0-420D-92C4-B4CB10EA683C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="30" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1663793" y="21997930"/>
+          <a:ext cx="738748" cy="369011"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>403410</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>107577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>452119</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>44357</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="직선 화살표 연결선 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E10A0E64-308A-4BF1-868A-EDEA7D42B1FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3487269" y="17956306"/>
+          <a:ext cx="48709" cy="3970898"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>269559</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>174348</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>632166</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>13602</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="타원 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A4C15FD-B461-4F03-A267-5F19C05DAA91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276783" y="17126607"/>
+          <a:ext cx="362607" cy="959842"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>579063</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>421341</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>90797</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="직선 화살표 연결선 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1CF63ED-B75B-4231-8719-F844FCF7998B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="38" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4586287" y="15777882"/>
+          <a:ext cx="765642" cy="1489291"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>568660</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>568660</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>215153</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="직선 화살표 연결선 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C1D60EA-381D-4A22-8D96-4EE64792AA92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3652519" y="17122588"/>
+          <a:ext cx="0" cy="941294"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>461084</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>197223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>461084</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>215152</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="직선 화살표 연결선 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B685DE27-B160-401C-8215-11D64AF49352}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3544943" y="15804776"/>
+          <a:ext cx="0" cy="2259105"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>269559</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>210207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>632166</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>49461</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="타원 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11176A61-60F6-494E-8FFE-28D1C5AB7566}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7279959" y="16265995"/>
+          <a:ext cx="362607" cy="959842"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>579063</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>133012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="직선 화살표 연결선 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{977F3F43-D61D-472B-96D2-D7BD0DAA6F92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7589463" y="17085271"/>
+          <a:ext cx="451878" cy="5308564"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>443155</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>188258</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>443155</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="직선 화살표 연결선 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A6E2948-2567-4426-AE17-3A634309A82D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6575014" y="16244046"/>
+          <a:ext cx="0" cy="851648"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2518,11 +3145,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7F5043-D2E6-404E-B1EC-48444BC9E7CF}">
-  <dimension ref="B1:L105"/>
+  <dimension ref="B1:L100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -2540,21 +3165,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="F2" s="11" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="F2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="J2" s="11" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="J2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
@@ -2614,9 +3239,9 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="1"/>
@@ -2635,9 +3260,9 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
       <c r="F7" s="1"/>
       <c r="G7" s="6" t="s">
         <v>6</v>
@@ -2654,9 +3279,9 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
       <c r="F8" s="1"/>
       <c r="G8" s="6" t="s">
         <v>7</v>
@@ -2673,9 +3298,9 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
       <c r="F9" s="1" t="s">
         <v>3</v>
       </c>
@@ -2686,7 +3311,7 @@
         <v>9</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>4</v>
@@ -2696,100 +3321,100 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16" t="s">
+      <c r="J10" s="11"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L11" s="19">
+      <c r="L11" s="16">
         <v>8048421</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="18" t="s">
+      <c r="J12" s="14"/>
+      <c r="K12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="16">
         <v>8048420</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="18">
         <v>55</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="18">
         <v>89</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="18">
         <v>83</v>
       </c>
-      <c r="L13" s="22" t="s">
+      <c r="L13" s="19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="F15" s="11" t="s">
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="F15" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
-      <c r="J15" s="11" t="s">
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="J15" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
@@ -2937,15 +3562,15 @@
         <v>13</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="25"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1"/>
@@ -2960,9 +3585,9 @@
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
       <c r="F24" s="1"/>
       <c r="G24" s="6"/>
       <c r="H24" s="2"/>
@@ -2975,9 +3600,9 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
       <c r="F25" s="1"/>
       <c r="G25" s="6"/>
       <c r="H25" s="2"/>
@@ -2990,9 +3615,9 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
       <c r="F26" s="1"/>
       <c r="G26" s="6"/>
       <c r="H26" s="2"/>
@@ -3005,9 +3630,9 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
       <c r="F27" s="1"/>
       <c r="G27" s="6"/>
       <c r="H27" s="2"/>
@@ -3022,9 +3647,9 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
       <c r="F28" s="1"/>
       <c r="G28" s="6"/>
       <c r="H28" s="2" t="s">
@@ -3037,9 +3662,9 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
       <c r="F29" s="1" t="s">
         <v>3</v>
       </c>
@@ -3056,191 +3681,191 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="16" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="14"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="16" t="s">
+      <c r="J30" s="11"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="23" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="17"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="19"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="16"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="23" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J32" s="17"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="19"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="16"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="23" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="17"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="19"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="16"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="16">
         <v>8048429</v>
       </c>
-      <c r="J34" s="17"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="19"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="16"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18" t="s">
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H35" s="16">
         <v>8048428</v>
       </c>
-      <c r="J35" s="17"/>
-      <c r="K35" s="18" t="s">
+      <c r="J35" s="14"/>
+      <c r="K35" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="L35" s="19">
+      <c r="L35" s="16">
         <v>8048430</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B36" s="17"/>
-      <c r="C36" s="18">
+      <c r="B36" s="14"/>
+      <c r="C36" s="15">
         <v>20</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="16">
         <v>8048424</v>
       </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="18">
+      <c r="F36" s="14"/>
+      <c r="G36" s="15">
         <v>24</v>
       </c>
-      <c r="H36" s="19">
+      <c r="H36" s="16">
         <v>8048427</v>
       </c>
-      <c r="J36" s="17"/>
-      <c r="K36" s="18">
+      <c r="J36" s="14"/>
+      <c r="K36" s="15">
         <v>24</v>
       </c>
-      <c r="L36" s="19" t="s">
+      <c r="L36" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B37" s="17"/>
-      <c r="C37" s="18" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="16">
         <v>8048423</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18">
+      <c r="F37" s="14"/>
+      <c r="G37" s="15">
         <v>44</v>
       </c>
-      <c r="H37" s="19">
+      <c r="H37" s="16">
         <v>8048426</v>
       </c>
-      <c r="J37" s="17"/>
-      <c r="K37" s="18">
+      <c r="J37" s="14"/>
+      <c r="K37" s="15">
         <v>44</v>
       </c>
-      <c r="L37" s="19" t="s">
+      <c r="L37" s="16" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="38" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="18">
         <v>83</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="19">
         <v>8048422</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H38" s="22">
+      <c r="H38" s="19">
         <v>8048425</v>
       </c>
-      <c r="J38" s="20" t="s">
+      <c r="J38" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K38" s="21" t="s">
+      <c r="K38" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="L38" s="22" t="s">
+      <c r="L38" s="19" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="40" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="F40" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="13"/>
-      <c r="J40" s="11" t="s">
+      <c r="C40" s="24"/>
+      <c r="D40" s="25"/>
+      <c r="F40" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" s="24"/>
+      <c r="H40" s="25"/>
+      <c r="J40" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="K40" s="12"/>
-      <c r="L40" s="13"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="25"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B41" s="1"/>
@@ -3642,192 +4267,192 @@
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B60" s="14"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="16" t="s">
+      <c r="B60" s="11"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="14"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="16" t="s">
+      <c r="F60" s="11"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J60" s="14"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="16" t="s">
+      <c r="J60" s="11"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B61" s="17"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="19"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="23" t="s">
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="16"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H61" s="19" t="s">
+      <c r="H61" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J61" s="17"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="19"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="16"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B62" s="17"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="19"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="23" t="s">
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="16"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H62" s="19" t="s">
+      <c r="H62" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="J62" s="17" t="s">
+      <c r="J62" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K62" s="18" t="s">
+      <c r="K62" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="L62" s="19">
+      <c r="L62" s="16">
         <v>8048441</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="19"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="18">
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="16"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="15">
         <v>84</v>
       </c>
-      <c r="H63" s="19">
+      <c r="H63" s="16">
         <v>8048439</v>
       </c>
-      <c r="J63" s="17"/>
-      <c r="K63" s="18" t="s">
+      <c r="J63" s="14"/>
+      <c r="K63" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L63" s="19">
+      <c r="L63" s="16">
         <v>8048440</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B64" s="17"/>
-      <c r="C64" s="23" t="s">
+      <c r="B64" s="14"/>
+      <c r="C64" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="19">
+      <c r="D64" s="16">
         <v>8048434</v>
       </c>
-      <c r="F64" s="17"/>
-      <c r="G64" s="18" t="s">
+      <c r="F64" s="14"/>
+      <c r="G64" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H64" s="19">
+      <c r="H64" s="16">
         <v>8048438</v>
       </c>
-      <c r="J64" s="17"/>
-      <c r="K64" s="18" t="s">
+      <c r="J64" s="14"/>
+      <c r="K64" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L64" s="19" t="s">
+      <c r="L64" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B65" s="17"/>
-      <c r="C65" s="18">
+      <c r="B65" s="14"/>
+      <c r="C65" s="15">
         <v>24</v>
       </c>
-      <c r="D65" s="19">
+      <c r="D65" s="16">
         <v>8048433</v>
       </c>
-      <c r="F65" s="17"/>
-      <c r="G65" s="18">
+      <c r="F65" s="14"/>
+      <c r="G65" s="15">
         <v>24</v>
       </c>
-      <c r="H65" s="19">
+      <c r="H65" s="16">
         <v>8048437</v>
       </c>
-      <c r="J65" s="17"/>
-      <c r="K65" s="18" t="s">
+      <c r="J65" s="14"/>
+      <c r="K65" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="L65" s="19" t="s">
+      <c r="L65" s="16" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B66" s="17"/>
-      <c r="C66" s="18">
+      <c r="B66" s="14"/>
+      <c r="C66" s="15">
         <v>44</v>
       </c>
-      <c r="D66" s="19">
+      <c r="D66" s="16">
         <v>8048432</v>
       </c>
-      <c r="F66" s="17"/>
-      <c r="G66" s="23" t="s">
+      <c r="F66" s="14"/>
+      <c r="G66" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H66" s="19">
+      <c r="H66" s="16">
         <v>8048436</v>
       </c>
-      <c r="J66" s="17"/>
-      <c r="K66" s="18" t="s">
+      <c r="J66" s="14"/>
+      <c r="K66" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="L66" s="19" t="s">
+      <c r="L66" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="67" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="21">
+      <c r="C67" s="18">
         <v>89</v>
       </c>
-      <c r="D67" s="22">
+      <c r="D67" s="19">
         <v>8048431</v>
       </c>
-      <c r="F67" s="20" t="s">
+      <c r="F67" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G67" s="21" t="s">
+      <c r="G67" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H67" s="22">
+      <c r="H67" s="19">
         <v>8048435</v>
       </c>
-      <c r="J67" s="20" t="s">
+      <c r="J67" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K67" s="21" t="s">
+      <c r="K67" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="L67" s="22" t="s">
+      <c r="L67" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="68" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="69" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C69" s="12"/>
-      <c r="D69" s="13"/>
-      <c r="F69" s="11" t="s">
+      <c r="C69" s="24"/>
+      <c r="D69" s="25"/>
+      <c r="F69" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G69" s="24"/>
+      <c r="H69" s="25"/>
+      <c r="J69" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="12"/>
-      <c r="H69" s="13"/>
-      <c r="J69" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="K69" s="12"/>
-      <c r="L69" s="13"/>
+      <c r="K69" s="24"/>
+      <c r="L69" s="25"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B70" s="1"/>
@@ -3875,7 +4500,7 @@
       </c>
       <c r="K72" s="6"/>
       <c r="L72" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.4">
@@ -3886,9 +4511,11 @@
       <c r="G73" s="6"/>
       <c r="H73" s="2"/>
       <c r="J73" s="1"/>
-      <c r="K73" s="6"/>
+      <c r="K73" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="L73" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.4">
@@ -3899,9 +4526,11 @@
       <c r="G74" s="6"/>
       <c r="H74" s="2"/>
       <c r="J74" s="1"/>
-      <c r="K74" s="6"/>
+      <c r="K74" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="L74" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.4">
@@ -3912,9 +4541,11 @@
       <c r="G75" s="6"/>
       <c r="H75" s="2"/>
       <c r="J75" s="1"/>
-      <c r="K75" s="6"/>
+      <c r="K75" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="L75" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.4">
@@ -3931,7 +4562,9 @@
         <v>0</v>
       </c>
       <c r="J76" s="1"/>
-      <c r="K76" s="6"/>
+      <c r="K76" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="L76" s="2" t="s">
         <v>0</v>
       </c>
@@ -4441,124 +5074,49 @@
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B99" s="14"/>
-      <c r="C99" s="15"/>
-      <c r="D99" s="16" t="s">
+      <c r="B99" s="11"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F99" s="14"/>
-      <c r="G99" s="15"/>
-      <c r="H99" s="16" t="s">
+      <c r="F99" s="11"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J99" s="14"/>
-      <c r="K99" s="15"/>
-      <c r="L99" s="16" t="s">
+      <c r="J99" s="11"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B100" s="17"/>
-      <c r="C100" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D100" s="19" t="s">
+    <row r="100" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B100" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D100" s="19">
+        <v>8048441</v>
+      </c>
+      <c r="F100" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G100" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="H100" s="19">
+        <v>8048442</v>
+      </c>
+      <c r="J100" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K100" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F100" s="17"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="19"/>
-      <c r="J100" s="17"/>
-      <c r="K100" s="18"/>
-      <c r="L100" s="19"/>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B101" s="17"/>
-      <c r="C101" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D101" s="19" t="s">
+      <c r="L100" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="F101" s="17"/>
-      <c r="G101" s="23"/>
-      <c r="H101" s="19"/>
-      <c r="J101" s="17"/>
-      <c r="K101" s="18"/>
-      <c r="L101" s="19"/>
-    </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B102" s="17"/>
-      <c r="C102" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F102" s="17"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="19"/>
-      <c r="J102" s="17"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="19"/>
-    </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B103" s="17"/>
-      <c r="C103" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D103" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F103" s="17"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="19"/>
-      <c r="J103" s="17"/>
-      <c r="K103" s="18"/>
-      <c r="L103" s="19"/>
-    </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B104" s="17"/>
-      <c r="C104" s="18">
-        <v>25</v>
-      </c>
-      <c r="D104" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F104" s="17"/>
-      <c r="G104" s="18"/>
-      <c r="H104" s="19"/>
-      <c r="J104" s="17"/>
-      <c r="K104" s="18"/>
-      <c r="L104" s="19"/>
-    </row>
-    <row r="105" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B105" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C105" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D105" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F105" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G105" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="H105" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="J105" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="K105" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="L105" s="22" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4580,7 +5138,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="K56:K57 G31:G33 G61:G62 G66 C64 K91:K92 K95:K96 C91:C92 C95:C96 C100:C101 K24:K26 C47:C49 G47:G49 K47:K49 G82:G84 C82:C84 K82:K84 G91:G92 G95:G96" numberStoredAsText="1"/>
+    <ignoredError sqref="K56:K57 G31:G33 G61:G62 G66 C64 K91:K92 K95:K96 C91:C92 C95:C96 K24:K26 C47:C49 G47:G49 K47:K49 G82:G84 C82:C84 K82:K84 G91:G92 G95:G96" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
[1W-3] Done lect1 hw8
- Completed lect1 hw
- Revised memory map
(eax stores real data in this ex)
</commit_message>
<xml_diff>
--- a/lect01_hw3_memory map.xlsx
+++ b/lect01_hw3_memory map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inha0-my.sharepoint.com/personal/12161756_inha_edu/Documents/Git/Information_Security/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{BD0A9945-A229-40C2-805E-F4872CD8B0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46DC22B3-7686-42F9-B730-BCC8BE93DD69}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{BD0A9945-A229-40C2-805E-F4872CD8B0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{520C7228-112B-4C20-B3C5-AF74A598D0B7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA8BD21B-3500-4B17-94FF-5435036B4A47}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="104">
   <si>
     <t>bffff63c</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>eax</t>
-  </si>
-  <si>
-    <t>eax</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -202,10 +199,6 @@
     <t>bffff62c</t>
   </si>
   <si>
-    <t>2c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bffff617</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -431,6 +424,14 @@
   </si>
   <si>
     <t>c3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>esp+0x4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +472,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,7 +666,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -736,6 +743,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1893,14 +1909,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>440931</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>107577</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>185057</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>451372</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>62285</xdr:rowOff>
+      <xdr:colOff>450392</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>62286</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1915,15 +1931,15 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3524790" y="12317506"/>
-          <a:ext cx="10441" cy="851179"/>
+          <a:off x="3554245" y="12300857"/>
+          <a:ext cx="9461" cy="748086"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:srgbClr val="FFC000"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -1948,81 +1964,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>278524</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>174348</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>641131</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>13602</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="72" name="타원 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62D3E87E-DBE8-4B40-A568-7F542A45CB53}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4285748" y="11487807"/>
-          <a:ext cx="362607" cy="959842"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:srgbClr val="FFC000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>588028</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>206188</xdr:rowOff>
+      <xdr:colOff>588030</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>394448</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>90797</xdr:rowOff>
+      <xdr:colOff>478972</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114283</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2034,20 +1984,21 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:endCxn id="72" idx="7"/>
+          <a:cxnSpLocks/>
+          <a:endCxn id="57" idx="7"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4595252" y="11295529"/>
-          <a:ext cx="729784" cy="332844"/>
+          <a:off x="4626630" y="9002486"/>
+          <a:ext cx="816228" cy="2574454"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="FFC000"/>
+            <a:srgbClr val="FFFF00"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -2073,13 +2024,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>260595</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>201243</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>623202</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>31532</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2104,7 +2055,7 @@
         <a:noFill/>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
+            <a:srgbClr val="00B050"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
@@ -2145,7 +2096,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>484095</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>117691</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2171,7 +2122,7 @@
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
+            <a:srgbClr val="00B050"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -2197,13 +2148,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>412377</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>412377</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>57187</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2253,13 +2204,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>233701</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>192278</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>596308</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>22567</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2319,13 +2270,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>543205</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>115083</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>439270</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>26894</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2377,13 +2328,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>403410</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>107577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>452119</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>44357</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2433,13 +2384,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>269559</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>174348</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>632166</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>13602</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2499,13 +2450,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>579063</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>170329</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>421341</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>90797</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2557,13 +2508,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>568660</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>170329</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>568660</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>215153</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2613,13 +2564,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>461084</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>197223</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>461084</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>215152</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2669,13 +2620,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>269559</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>210207</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>632166</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>49461</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2735,13 +2686,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>579063</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>133012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>53788</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2793,13 +2744,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>443155</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>188258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>443155</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>143435</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2843,6 +2794,196 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>234982</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>196120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>597589</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>35373</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="타원 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B0E5815-C988-4AE5-AD68-BE03B9CD0007}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1367096" y="10123891"/>
+          <a:ext cx="362607" cy="927825"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>544486</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>391886</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>114282</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="직선 화살표 연결선 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50265DE9-FD1B-49E2-985D-B5E84939B036}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="55" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1676600" y="8980714"/>
+          <a:ext cx="696486" cy="1507654"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>278526</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>196120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>641133</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>35373</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="타원 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BE3775C-6309-4CB7-B505-E2B415F090C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4317126" y="11441063"/>
+          <a:ext cx="362607" cy="927824"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3145,7 +3286,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7F5043-D2E6-404E-B1EC-48444BC9E7CF}">
-  <dimension ref="B1:L100"/>
+  <dimension ref="B1:L102"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -3311,7 +3452,7 @@
         <v>9</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>4</v>
@@ -3344,7 +3485,7 @@
       <c r="H11" s="16"/>
       <c r="J11" s="14"/>
       <c r="K11" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L11" s="16">
         <v>8048421</v>
@@ -3356,14 +3497,14 @@
       <c r="D12" s="16"/>
       <c r="F12" s="14"/>
       <c r="G12" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L12" s="16">
         <v>8048420</v>
@@ -3371,31 +3512,31 @@
     </row>
     <row r="13" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="18">
         <v>55</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G13" s="18">
         <v>89</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K13" s="18">
         <v>83</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
@@ -3411,7 +3552,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="25"/>
       <c r="J15" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K15" s="24"/>
       <c r="L15" s="25"/>
@@ -3593,7 +3734,7 @@
       <c r="H24" s="2"/>
       <c r="J24" s="1"/>
       <c r="K24" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>20</v>
@@ -3608,7 +3749,7 @@
       <c r="H25" s="2"/>
       <c r="J25" s="1"/>
       <c r="K25" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>21</v>
@@ -3623,7 +3764,7 @@
       <c r="H26" s="2"/>
       <c r="J26" s="1"/>
       <c r="K26" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>22</v>
@@ -3701,10 +3842,10 @@
       <c r="D31" s="16"/>
       <c r="F31" s="14"/>
       <c r="G31" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="15"/>
@@ -3716,10 +3857,10 @@
       <c r="D32" s="16"/>
       <c r="F32" s="14"/>
       <c r="G32" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="15"/>
@@ -3731,10 +3872,10 @@
       <c r="D33" s="16"/>
       <c r="F33" s="14"/>
       <c r="G33" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J33" s="14"/>
       <c r="K33" s="15"/>
@@ -3761,14 +3902,14 @@
       <c r="D35" s="16"/>
       <c r="F35" s="14"/>
       <c r="G35" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H35" s="16">
         <v>8048428</v>
       </c>
       <c r="J35" s="14"/>
       <c r="K35" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L35" s="16">
         <v>8048430</v>
@@ -3794,13 +3935,13 @@
         <v>24</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B37" s="14"/>
       <c r="C37" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37" s="16">
         <v>8048423</v>
@@ -3817,12 +3958,12 @@
         <v>44</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B38" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="18">
         <v>83</v>
@@ -3831,22 +3972,22 @@
         <v>8048422</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H38" s="19">
         <v>8048425</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K38" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
@@ -3857,280 +3998,284 @@
       <c r="C40" s="24"/>
       <c r="D40" s="25"/>
       <c r="F40" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G40" s="24"/>
       <c r="H40" s="25"/>
       <c r="J40" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K40" s="24"/>
       <c r="L40" s="25"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B41" s="1"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J41" s="1"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="2" t="s">
-        <v>27</v>
+    <row r="41" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="27"/>
+      <c r="H41" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K41" s="27"/>
+      <c r="L41" s="28" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B42" s="1"/>
-      <c r="C42" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="C42" s="5"/>
       <c r="D42" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1"/>
-      <c r="G42" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="G42" s="5"/>
       <c r="H42" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="J42" s="1"/>
-      <c r="K42" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="K42" s="5"/>
       <c r="L42" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B43" s="1"/>
       <c r="C43" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B44" s="1"/>
       <c r="C44" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B45" s="1"/>
+      <c r="C45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L44" s="2" t="s">
+      <c r="J45" s="1"/>
+      <c r="K45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="G46" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="H46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J45" s="1" t="s">
+      <c r="J46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K46" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K45" s="6" t="s">
+      <c r="L46" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B46" s="1"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J46" s="1"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B47" s="1"/>
-      <c r="C47" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="C47" s="6"/>
       <c r="D47" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1"/>
-      <c r="G47" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="G47" s="6"/>
       <c r="H47" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J47" s="1"/>
-      <c r="K47" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="K47" s="6"/>
       <c r="L47" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B48" s="1"/>
       <c r="C48" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B49" s="1"/>
       <c r="C49" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L49" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B50" s="1"/>
+      <c r="C50" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J50" s="1"/>
+      <c r="K50" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B50" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G50" s="6" t="s">
+      <c r="H51" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K50" s="6" t="s">
+      <c r="J51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B51" s="1"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J51" s="1"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B52" s="1"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F52" s="1"/>
-      <c r="G52" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="G52" s="6"/>
       <c r="H52" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="J52" s="1"/>
-      <c r="K52" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="K52" s="6"/>
       <c r="L52" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.4">
@@ -4138,18 +4283,18 @@
       <c r="C53" s="6"/>
       <c r="D53" s="2"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="6" t="s">
-        <v>6</v>
+      <c r="G53" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J53" s="1"/>
-      <c r="K53" s="6" t="s">
-        <v>6</v>
+      <c r="K53" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.4">
@@ -4157,18 +4302,18 @@
       <c r="C54" s="6"/>
       <c r="D54" s="2"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="6" t="s">
-        <v>7</v>
+      <c r="G54" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="K54" s="6" t="s">
-        <v>7</v>
+      <c r="K54" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.4">
@@ -4176,35 +4321,39 @@
       <c r="C55" s="6"/>
       <c r="D55" s="2"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="6" t="s">
-        <v>46</v>
+      <c r="G55" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J55" s="1"/>
-      <c r="K55" s="6" t="s">
-        <v>46</v>
+      <c r="K55" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B56" s="1"/>
       <c r="C56" s="6"/>
       <c r="D56" s="2"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="6"/>
+      <c r="F56" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="H56" s="2" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="J56" s="1"/>
-      <c r="K56" s="9" t="s">
-        <v>54</v>
+      <c r="K56" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.4">
@@ -4213,90 +4362,92 @@
       <c r="D57" s="2"/>
       <c r="F57" s="1"/>
       <c r="G57" s="6"/>
-      <c r="H57" s="2"/>
+      <c r="H57" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J57" s="1"/>
       <c r="K57" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B58" s="1"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="D58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="6"/>
-      <c r="H58" s="2" t="s">
+      <c r="H58" s="2"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B59" s="1"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J58" s="1"/>
-      <c r="K58" s="6">
+      <c r="F59" s="1"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J59" s="1"/>
+      <c r="K59" s="6">
         <v>84</v>
       </c>
-      <c r="L58" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="1" t="s">
+      <c r="L59" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="2" t="s">
+      <c r="C60" s="10"/>
+      <c r="D60" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G59" s="10"/>
-      <c r="H59" s="2" t="s">
+      <c r="G60" s="10"/>
+      <c r="H60" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K59" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L59" s="2" t="s">
+      <c r="K60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L60" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B60" s="11"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="13" t="s">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B61" s="11"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="11"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="13" t="s">
+      <c r="F61" s="11"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J60" s="11"/>
-      <c r="K60" s="12"/>
-      <c r="L60" s="13" t="s">
+      <c r="J61" s="11"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B61" s="14"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="16"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H61" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J61" s="14"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="16"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B62" s="14"/>
@@ -4304,203 +4455,211 @@
       <c r="D62" s="16"/>
       <c r="F62" s="14"/>
       <c r="G62" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="J62" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="K62" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="L62" s="16">
-        <v>8048441</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="J62" s="14"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="16"/>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B63" s="14"/>
       <c r="C63" s="15"/>
       <c r="D63" s="16"/>
       <c r="F63" s="14"/>
-      <c r="G63" s="15">
-        <v>84</v>
-      </c>
-      <c r="H63" s="16">
-        <v>8048439</v>
-      </c>
-      <c r="J63" s="14"/>
+      <c r="G63" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J63" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="K63" s="15" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="L63" s="16">
-        <v>8048440</v>
+        <v>8048441</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B64" s="14"/>
-      <c r="C64" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" s="16">
-        <v>8048434</v>
-      </c>
+      <c r="C64" s="15"/>
+      <c r="D64" s="16"/>
       <c r="F64" s="14"/>
-      <c r="G64" s="15" t="s">
-        <v>53</v>
+      <c r="G64" s="15">
+        <v>84</v>
       </c>
       <c r="H64" s="16">
-        <v>8048438</v>
+        <v>8048439</v>
       </c>
       <c r="J64" s="14"/>
       <c r="K64" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L64" s="16" t="s">
-        <v>90</v>
+      <c r="L64" s="16">
+        <v>8048440</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B65" s="14"/>
-      <c r="C65" s="15">
-        <v>24</v>
+      <c r="C65" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="D65" s="16">
-        <v>8048433</v>
+        <v>8048434</v>
       </c>
       <c r="F65" s="14"/>
-      <c r="G65" s="15">
-        <v>24</v>
+      <c r="G65" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="H65" s="16">
-        <v>8048437</v>
+        <v>8048438</v>
       </c>
       <c r="J65" s="14"/>
       <c r="K65" s="15" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
       <c r="L65" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B66" s="14"/>
       <c r="C66" s="15">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D66" s="16">
-        <v>8048432</v>
+        <v>8048433</v>
       </c>
       <c r="F66" s="14"/>
-      <c r="G66" s="20" t="s">
-        <v>55</v>
+      <c r="G66" s="15">
+        <v>24</v>
       </c>
       <c r="H66" s="16">
-        <v>8048436</v>
+        <v>8048437</v>
       </c>
       <c r="J66" s="14"/>
       <c r="K66" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L66" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B67" s="14"/>
+      <c r="C67" s="15">
+        <v>44</v>
+      </c>
+      <c r="D67" s="16">
+        <v>8048432</v>
+      </c>
+      <c r="F67" s="14"/>
+      <c r="G67" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H67" s="16">
+        <v>8048436</v>
+      </c>
+      <c r="J67" s="14"/>
+      <c r="K67" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="L67" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B68" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="18">
+        <v>89</v>
+      </c>
+      <c r="D68" s="19">
+        <v>8048431</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H68" s="19">
+        <v>8048435</v>
+      </c>
+      <c r="J68" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="K68" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L68" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="L66" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B67" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" s="18">
-        <v>89</v>
-      </c>
-      <c r="D67" s="19">
-        <v>8048431</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H67" s="19">
-        <v>8048435</v>
-      </c>
-      <c r="J67" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K67" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="L67" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="69" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B69" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="24"/>
-      <c r="D69" s="25"/>
-      <c r="F69" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G69" s="24"/>
-      <c r="H69" s="25"/>
-      <c r="J69" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="K69" s="24"/>
-      <c r="L69" s="25"/>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B70" s="1"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="2"/>
-      <c r="F70" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K70" s="7"/>
-      <c r="L70" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B71" s="1"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="2"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J71" s="1"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="2" t="s">
-        <v>12</v>
+    </row>
+    <row r="69" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="70" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B70" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" s="24"/>
+      <c r="D70" s="25"/>
+      <c r="F70" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="G70" s="24"/>
+      <c r="H70" s="25"/>
+      <c r="J70" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K70" s="24"/>
+      <c r="L70" s="25"/>
+    </row>
+    <row r="71" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B71" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="27"/>
+      <c r="D71" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" s="27"/>
+      <c r="H71" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J71" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K71" s="27"/>
+      <c r="L71" s="28" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B72" s="1"/>
-      <c r="C72" s="6"/>
+      <c r="C72" s="5"/>
       <c r="D72" s="2"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="6"/>
-      <c r="H72" s="2"/>
-      <c r="J72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K72" s="6"/>
-      <c r="L72" s="2" t="s">
-        <v>95</v>
+      <c r="F72" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G72" s="7"/>
+      <c r="H72" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K72" s="7"/>
+      <c r="L72" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.4">
@@ -4509,13 +4668,13 @@
       <c r="D73" s="2"/>
       <c r="F73" s="1"/>
       <c r="G73" s="6"/>
-      <c r="H73" s="2"/>
+      <c r="H73" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J73" s="1"/>
-      <c r="K73" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="K73" s="6"/>
       <c r="L73" s="2" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.4">
@@ -4525,12 +4684,12 @@
       <c r="F74" s="1"/>
       <c r="G74" s="6"/>
       <c r="H74" s="2"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="J74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K74" s="6"/>
       <c r="L74" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.4">
@@ -4542,7 +4701,7 @@
       <c r="H75" s="2"/>
       <c r="J75" s="1"/>
       <c r="K75" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>96</v>
@@ -4550,595 +4709,625 @@
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B76" s="1"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="2"/>
+      <c r="F76" s="1"/>
       <c r="G76" s="6"/>
-      <c r="H76" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="H76" s="2"/>
       <c r="J76" s="1"/>
       <c r="K76" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B77" s="1"/>
-      <c r="C77" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="2"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="G77" s="6"/>
+      <c r="H77" s="2"/>
       <c r="J77" s="1"/>
       <c r="K77" s="6" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B78" s="1"/>
-      <c r="C78" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="C78" s="5"/>
       <c r="D78" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F78" s="1"/>
-      <c r="G78" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G78" s="6"/>
       <c r="H78" s="2" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="6" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B79" s="1"/>
       <c r="C79" s="6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J79" s="1"/>
       <c r="K79" s="6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B80" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="B80" s="1"/>
       <c r="C80" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J80" s="1"/>
       <c r="K80" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B81" s="1"/>
-      <c r="C81" s="6"/>
+      <c r="C81" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D81" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F81" s="1"/>
-      <c r="G81" s="6"/>
+      <c r="G81" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H81" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J81" s="1"/>
-      <c r="K81" s="6"/>
+      <c r="K81" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="L81" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B82" s="1"/>
-      <c r="C82" s="9" t="s">
-        <v>73</v>
+      <c r="B82" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F82" s="1"/>
-      <c r="G82" s="9" t="s">
-        <v>73</v>
+      <c r="G82" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J82" s="1"/>
-      <c r="K82" s="9" t="s">
-        <v>73</v>
+      <c r="K82" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B83" s="1"/>
-      <c r="C83" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="C83" s="6"/>
       <c r="D83" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F83" s="1"/>
-      <c r="G83" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="G83" s="6"/>
       <c r="H83" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="J83" s="1"/>
-      <c r="K83" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="K83" s="6"/>
       <c r="L83" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B84" s="1"/>
       <c r="C84" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J84" s="1"/>
       <c r="K84" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B85" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>44</v>
+      <c r="B85" s="1"/>
+      <c r="C85" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="F85" s="1"/>
+      <c r="G85" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J85" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K85" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="J85" s="1"/>
+      <c r="K85" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B86" s="1"/>
-      <c r="C86" s="6"/>
+      <c r="C86" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="D86" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F86" s="1"/>
-      <c r="G86" s="6"/>
+      <c r="G86" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="H86" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="J86" s="1"/>
-      <c r="K86" s="6"/>
+      <c r="K86" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="L86" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B87" s="1"/>
       <c r="C87" s="6" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="6" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="6" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B88" s="1"/>
-      <c r="C88" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C88" s="6"/>
       <c r="D88" s="2" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F88" s="1"/>
-      <c r="G88" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="G88" s="6"/>
       <c r="H88" s="2" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="J88" s="1"/>
-      <c r="K88" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="K88" s="6"/>
       <c r="L88" s="2" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B89" s="1"/>
-      <c r="C89" s="6" t="s">
-        <v>7</v>
+      <c r="C89" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F89" s="1"/>
-      <c r="G89" s="6" t="s">
-        <v>7</v>
+      <c r="G89" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J89" s="1"/>
-      <c r="K89" s="6" t="s">
-        <v>7</v>
+      <c r="K89" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B90" s="1"/>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="F90" s="1"/>
-      <c r="G90" s="6" t="s">
+      <c r="G90" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H90" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H90" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="J90" s="1"/>
-      <c r="K90" s="6" t="s">
+      <c r="K90" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="L90" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="L90" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B91" s="1"/>
       <c r="C91" s="9" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="9" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="9" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B92" s="1"/>
-      <c r="C92" s="9" t="s">
-        <v>55</v>
+      <c r="C92" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F92" s="1"/>
-      <c r="G92" s="9" t="s">
-        <v>55</v>
+      <c r="G92" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="J92" s="1"/>
-      <c r="K92" s="9" t="s">
-        <v>55</v>
+      <c r="K92" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B93" s="1"/>
-      <c r="C93" s="6">
-        <v>84</v>
+      <c r="C93" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F93" s="1"/>
-      <c r="G93" s="6">
-        <v>84</v>
+      <c r="G93" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J93" s="1"/>
-      <c r="K93" s="6">
-        <v>84</v>
+      <c r="K93" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B94" s="1"/>
-      <c r="C94" s="6" t="s">
+      <c r="C94" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="F94" s="1"/>
-      <c r="G94" s="6" t="s">
+      <c r="G94" s="9" t="s">
         <v>53</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="J94" s="1"/>
-      <c r="K94" s="6" t="s">
+      <c r="K94" s="9" t="s">
         <v>53</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B95" s="1"/>
-      <c r="C95" s="9" t="s">
-        <v>54</v>
+      <c r="C95" s="6">
+        <v>84</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F95" s="1"/>
-      <c r="G95" s="9" t="s">
-        <v>54</v>
+      <c r="G95" s="6">
+        <v>84</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J95" s="1"/>
-      <c r="K95" s="9" t="s">
-        <v>54</v>
+      <c r="K95" s="6">
+        <v>84</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B96" s="1"/>
-      <c r="C96" s="9" t="s">
-        <v>55</v>
+      <c r="C96" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="F96" s="1"/>
-      <c r="G96" s="9" t="s">
-        <v>55</v>
+      <c r="G96" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J96" s="1"/>
-      <c r="K96" s="9" t="s">
-        <v>55</v>
+      <c r="K96" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B97" s="1"/>
-      <c r="C97" s="6">
+      <c r="C97" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F97" s="1"/>
+      <c r="G97" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J97" s="1"/>
+      <c r="K97" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B98" s="1"/>
+      <c r="C98" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F98" s="1"/>
+      <c r="G98" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J98" s="1"/>
+      <c r="K98" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B99" s="1"/>
+      <c r="C99" s="6">
         <v>84</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D99" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F99" s="1"/>
+      <c r="G99" s="6">
+        <v>84</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J99" s="1"/>
+      <c r="K99" s="6">
+        <v>84</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="10">
+        <v>41</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F100" s="1"/>
+      <c r="G100" s="10">
+        <v>41</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J100" s="1"/>
+      <c r="K100" s="10">
+        <v>41</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B101" s="11"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="11"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J101" s="11"/>
+      <c r="K101" s="12"/>
+      <c r="L101" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B102" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F97" s="1"/>
-      <c r="G97" s="6">
-        <v>84</v>
-      </c>
-      <c r="H97" s="2" t="s">
+      <c r="C102" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D102" s="19">
+        <v>8048441</v>
+      </c>
+      <c r="F102" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="J97" s="1"/>
-      <c r="K97" s="6">
-        <v>84</v>
-      </c>
-      <c r="L97" s="2" t="s">
+      <c r="G102" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H102" s="19">
+        <v>8048442</v>
+      </c>
+      <c r="J102" s="17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="98" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B98" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C98" s="10">
-        <v>41</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F98" s="1"/>
-      <c r="G98" s="10">
-        <v>41</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J98" s="1"/>
-      <c r="K98" s="10">
-        <v>41</v>
-      </c>
-      <c r="L98" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B99" s="11"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F99" s="11"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J99" s="11"/>
-      <c r="K99" s="12"/>
-      <c r="L99" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B100" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C100" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D100" s="19">
-        <v>8048441</v>
-      </c>
-      <c r="F100" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G100" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H100" s="19">
-        <v>8048442</v>
-      </c>
-      <c r="J100" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K100" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="L100" s="19" t="s">
-        <v>100</v>
+      <c r="K102" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="L102" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="J71:K71"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
     <mergeCell ref="J40:L40"/>
-    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="J15:L15"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="J69:L69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="J70:L70"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="J41:K41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="K56:K57 G31:G33 G61:G62 G66 C64 K91:K92 K95:K96 C91:C92 C95:C96 K24:K26 C47:C49 G47:G49 K47:K49 G82:G84 C82:C84 K82:K84 G91:G92 G95:G96" numberStoredAsText="1"/>
+    <ignoredError sqref="K57:K58 G31:G33 G62:G63 G67 C65 K93:K94 K97:K98 C93:C94 C97:C98 K24:K26 C48:C50 G48:G50 K48:K50 G84:G86 C84:C86 K84:K86 G93:G94 G97:G98 G53:G56 K53:K56 K89:K92 G89:G92 C89:C92" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>